<commit_message>
added ref999 jump results
</commit_message>
<xml_diff>
--- a/results/VRE_resource_summary_reseamed_years.xlsx
+++ b/results/VRE_resource_summary_reseamed_years.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonathan\git\PhD\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\129.16.54.22\Users\jonathan\git\PhD\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D383208-C24F-49BC-BFBB-BD305D93928D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3540" windowWidth="28800" windowHeight="14295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23385" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$65:$D$75</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="62">
   <si>
     <t>pot_cap</t>
   </si>
@@ -217,11 +219,14 @@
   <si>
     <t>Solar</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -248,12 +253,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -283,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -299,6 +310,18 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,11 +623,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:AQ75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="AN42" sqref="AN42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +1023,7 @@
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1127,7 +1151,7 @@
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="4" t="s">
         <v>45</v>
       </c>
@@ -1253,7 +1277,7 @@
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="4" t="s">
         <v>46</v>
       </c>
@@ -1379,7 +1403,7 @@
       </c>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="4" t="s">
         <v>47</v>
       </c>
@@ -1505,7 +1529,7 @@
       </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="4" t="s">
         <v>48</v>
       </c>
@@ -1631,7 +1655,7 @@
       </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
         <v>41</v>
       </c>
@@ -1757,7 +1781,7 @@
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1885,7 +1909,7 @@
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="4" t="s">
         <v>45</v>
       </c>
@@ -2011,7 +2035,7 @@
       </c>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="4" t="s">
         <v>46</v>
       </c>
@@ -2137,7 +2161,7 @@
       </c>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="4" t="s">
         <v>47</v>
       </c>
@@ -2263,7 +2287,7 @@
       </c>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="4" t="s">
         <v>48</v>
       </c>
@@ -2389,7 +2413,7 @@
       </c>
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
@@ -2515,7 +2539,7 @@
       </c>
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2643,7 +2667,7 @@
       </c>
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="4" t="s">
         <v>45</v>
       </c>
@@ -2769,7 +2793,7 @@
       </c>
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="4" t="s">
         <v>47</v>
       </c>
@@ -2895,7 +2919,7 @@
       </c>
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="4" t="s">
         <v>48</v>
       </c>
@@ -3149,7 +3173,7 @@
       </c>
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -3277,7 +3301,7 @@
       </c>
     </row>
     <row r="22" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="4" t="s">
         <v>47</v>
       </c>
@@ -3403,7 +3427,7 @@
       </c>
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -3531,7 +3555,7 @@
       </c>
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="4" t="s">
         <v>46</v>
       </c>
@@ -3657,7 +3681,7 @@
       </c>
     </row>
     <row r="25" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="4" t="s">
         <v>47</v>
       </c>
@@ -3783,7 +3807,7 @@
       </c>
     </row>
     <row r="26" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="4" t="s">
         <v>48</v>
       </c>
@@ -3909,7 +3933,7 @@
       </c>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -4037,7 +4061,7 @@
       </c>
     </row>
     <row r="28" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="4" t="s">
         <v>45</v>
       </c>
@@ -4163,7 +4187,7 @@
       </c>
     </row>
     <row r="29" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="4" t="s">
         <v>47</v>
       </c>
@@ -4289,7 +4313,7 @@
       </c>
     </row>
     <row r="30" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="4" t="s">
         <v>48</v>
       </c>
@@ -4415,7 +4439,7 @@
       </c>
     </row>
     <row r="31" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="4" t="s">
         <v>41</v>
       </c>
@@ -4541,7 +4565,7 @@
       </c>
     </row>
     <row r="32" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -4669,7 +4693,7 @@
       </c>
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="4" t="s">
         <v>46</v>
       </c>
@@ -4795,7 +4819,7 @@
       </c>
     </row>
     <row r="34" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="4" t="s">
         <v>47</v>
       </c>
@@ -4921,7 +4945,7 @@
       </c>
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="4" t="s">
         <v>48</v>
       </c>
@@ -5047,7 +5071,7 @@
       </c>
     </row>
     <row r="36" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="4" t="s">
         <v>41</v>
       </c>
@@ -5171,6 +5195,67 @@
       <c r="AP36" s="2">
         <v>1494.4383</v>
       </c>
+    </row>
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="N37" s="10"/>
+      <c r="O37" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="P37" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="S37" s="10"/>
+      <c r="T37" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="U37" s="10"/>
+      <c r="V37" s="10"/>
+      <c r="W37" s="10"/>
+      <c r="X37" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y37" s="10"/>
+      <c r="Z37" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA37" s="10"/>
+      <c r="AB37" s="10"/>
+      <c r="AC37" s="10"/>
+      <c r="AD37" s="10"/>
+      <c r="AE37" s="10"/>
+      <c r="AF37" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG37" s="10"/>
+      <c r="AH37" s="10"/>
+      <c r="AI37" s="10"/>
+      <c r="AJ37" s="10"/>
+      <c r="AK37" s="10"/>
+      <c r="AL37" s="10"/>
+      <c r="AM37" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN37" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO37" s="10"/>
+      <c r="AP37" s="10"/>
     </row>
     <row r="38" spans="1:43" x14ac:dyDescent="0.25">
       <c r="D38" s="4" t="s">
@@ -6306,7 +6391,7 @@
         <v>87.472267285065527</v>
       </c>
     </row>
-    <row r="49" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:42" x14ac:dyDescent="0.25">
       <c r="Q49" t="s">
         <v>59</v>
       </c>
@@ -6314,7 +6399,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:42" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
         <f t="shared" ref="D50:L50" si="6">D40-$M$40</f>
         <v>0.96601563371700649</v>
@@ -6472,7 +6557,7 @@
         <v>9.1374044521828637</v>
       </c>
     </row>
-    <row r="51" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:42" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
         <f t="shared" ref="D51:L51" si="8">D43-$M$43</f>
         <v>-61.728131587547068</v>
@@ -6630,7 +6715,198 @@
         <v>49.378939045722973</v>
       </c>
     </row>
+    <row r="54" spans="3:42" x14ac:dyDescent="0.25">
+      <c r="M54" s="6">
+        <f>M46</f>
+        <v>28.955923787160145</v>
+      </c>
+      <c r="O54" s="6">
+        <f>O46</f>
+        <v>23.755622382202773</v>
+      </c>
+      <c r="P54" s="6">
+        <f>P46</f>
+        <v>26.920373637537296</v>
+      </c>
+      <c r="R54" s="6">
+        <f>R46</f>
+        <v>47.216219374967523</v>
+      </c>
+      <c r="T54" s="6">
+        <f>T46</f>
+        <v>-15.854270236980028</v>
+      </c>
+      <c r="X54" s="6">
+        <f>X46</f>
+        <v>-53.22034296686661</v>
+      </c>
+      <c r="Z54" s="6">
+        <f>Z46</f>
+        <v>-46.275090124768212</v>
+      </c>
+      <c r="AF54" s="6">
+        <f>AF46</f>
+        <v>-32.135885930981203</v>
+      </c>
+      <c r="AM54" s="6">
+        <f>AM46</f>
+        <v>-11.056970015459001</v>
+      </c>
+      <c r="AN54" s="6">
+        <f>AN46</f>
+        <v>21.143688384385086</v>
+      </c>
+    </row>
+    <row r="63" spans="3:42" x14ac:dyDescent="0.25">
+      <c r="C63" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L63" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="3:42" x14ac:dyDescent="0.25">
+      <c r="C64" s="6">
+        <v>28.955923787160145</v>
+      </c>
+      <c r="D64" s="6">
+        <v>23.755622382202773</v>
+      </c>
+      <c r="E64" s="6">
+        <v>26.920373637537296</v>
+      </c>
+      <c r="F64" s="6">
+        <v>47.216219374967523</v>
+      </c>
+      <c r="G64" s="6">
+        <v>-15.854270236980028</v>
+      </c>
+      <c r="H64" s="6">
+        <v>-53.22034296686661</v>
+      </c>
+      <c r="I64" s="6">
+        <v>-46.275090124768212</v>
+      </c>
+      <c r="J64" s="6">
+        <v>-32.135885930981203</v>
+      </c>
+      <c r="K64" s="6">
+        <v>-11.056970015459001</v>
+      </c>
+      <c r="L64" s="6">
+        <v>21.143688384385086</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C66" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D66" s="6">
+        <v>-53.22034296686661</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C67" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67" s="6">
+        <v>-46.275090124768212</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D68" s="6">
+        <v>-32.135885930981203</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="6">
+        <v>-15.854270236980028</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C70" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D70" s="6">
+        <v>-11.056970015459001</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C71" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D71" s="6">
+        <v>21.143688384385086</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C72" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="6">
+        <v>23.755622382202773</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C73" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" s="6">
+        <v>26.920373637537296</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C74" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" s="6">
+        <v>28.955923787160145</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C75" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="6">
+        <v>47.216219374967523</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="C65:D75">
+    <sortState ref="C66:D75">
+      <sortCondition ref="D65:D75"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A32:A36"/>
     <mergeCell ref="A21:A22"/>

</xml_diff>